<commit_message>
added home purchase calcs
</commit_message>
<xml_diff>
--- a/dev/test_calcs.xlsx
+++ b/dev/test_calcs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejwda\Google Drive\01-ejw-data-github\Public\Sim\sim-financials\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2ECEEF-BC24-43C7-BEB6-986CEDD4288B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A7A30C-2CA7-47D7-8004-9482AE0F3799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{CF5539ED-CB69-4B4C-A3DC-900C31F33A78}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{CF5539ED-CB69-4B4C-A3DC-900C31F33A78}"/>
   </bookViews>
   <sheets>
     <sheet name="Calcs" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="95">
   <si>
     <t>Utilities (27%)</t>
   </si>
@@ -321,6 +321,9 @@
   <si>
     <t>Keep up to $500,000 if lived in 2 of the past 5 years</t>
   </si>
+  <si>
+    <t>gi</t>
+  </si>
 </sst>
 </file>
 
@@ -354,12 +357,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -374,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -388,6 +397,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -706,23 +717,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97E6AC9F-978D-4ABB-A9E1-2C7FE8E14DCC}">
   <dimension ref="A2:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -730,7 +741,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -738,7 +749,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -746,7 +757,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -754,7 +765,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -762,7 +773,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -770,7 +781,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -778,7 +789,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -786,7 +797,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
@@ -795,12 +806,12 @@
         <v>506</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -808,7 +819,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -816,7 +827,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -825,12 +836,12 @@
         <v>205</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -838,7 +849,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -849,7 +860,7 @@
         <v>2.1899999999999999E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -857,7 +868,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
@@ -866,12 +877,12 @@
         <v>308</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G24" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>15</v>
       </c>
@@ -882,7 +893,7 @@
         <v>13850</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -896,7 +907,7 @@
         <v>27700</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -910,7 +921,7 @@
         <v>20800</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -918,7 +929,7 @@
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -929,7 +940,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>21</v>
       </c>
@@ -941,7 +952,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>25</v>
       </c>
@@ -956,7 +967,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>26</v>
       </c>
@@ -971,24 +982,24 @@
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B33" s="4">
-        <f>B30/(1-(1/(1+B28/12)^(B29*12)))*B28/12</f>
+        <f>(B30*B28/12)/(1-(1/(1+B28/12)^(B29*12)))</f>
         <v>1229.8497276986884</v>
       </c>
       <c r="G33" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G34" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>24</v>
       </c>
@@ -1000,7 +1011,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G36" t="s">
         <v>88</v>
       </c>
@@ -1008,7 +1019,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>29</v>
       </c>
@@ -1016,7 +1027,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>30</v>
       </c>
@@ -1025,7 +1036,7 @@
         <v>1554.4052832542438</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>31</v>
       </c>
@@ -1034,12 +1045,12 @@
         <v>500</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>32</v>
       </c>
@@ -1048,16 +1059,16 @@
         <v>1054.4052832542438</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="5"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>34</v>
       </c>
@@ -1065,7 +1076,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>33</v>
       </c>
@@ -1086,18 +1097,18 @@
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1108,7 +1119,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -1119,7 +1130,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1130,7 +1141,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -1141,7 +1152,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -1152,12 +1163,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -1168,7 +1179,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -1179,7 +1190,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -1187,12 +1198,12 @@
         <v>350</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -1200,7 +1211,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -1208,7 +1219,7 @@
         <v>12500</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -1216,12 +1227,12 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -1235,7 +1246,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -1249,7 +1260,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>55</v>
       </c>
@@ -1257,7 +1268,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>56</v>
       </c>
@@ -1268,12 +1279,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -1284,7 +1295,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -1295,7 +1306,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>58</v>
       </c>
@@ -1306,12 +1317,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -1319,7 +1330,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>64</v>
       </c>
@@ -1327,7 +1338,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>65</v>
       </c>
@@ -1351,17 +1362,17 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="57.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>89</v>
       </c>
@@ -1373,25 +1384,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED1C0CDA-6B9F-4A1C-A616-D80F03516A77}">
-  <dimension ref="A3:H369"/>
+  <dimension ref="A3:N369"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -1399,7 +1410,7 @@
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -1408,7 +1419,7 @@
         <v>250000.05535254901</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -1417,7 +1428,7 @@
         <v>892662.56577908678</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -1425,12 +1436,12 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>76</v>
       </c>
@@ -1452,8 +1463,11 @@
       <c r="H8" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="N8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -1464,7 +1478,7 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1496,7 +1510,7 @@
         <v>249655.56666666668</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1528,7 +1542,7 @@
         <v>249309.91346527779</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1560,7 +1574,7 @@
         <v>248963.0360754673</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1592,7 +1606,7 @@
         <v>248614.93016156793</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>5</v>
       </c>
@@ -1624,7 +1638,7 @@
         <v>248265.59137255681</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6</v>
       </c>
@@ -1656,7 +1670,7 @@
         <v>247915.01534200128</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>7</v>
       </c>
@@ -1688,7 +1702,7 @@
         <v>247563.19768800421</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>8</v>
       </c>
@@ -1720,7 +1734,7 @@
         <v>247210.13401314922</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>9</v>
       </c>
@@ -1752,7 +1766,7 @@
         <v>246855.81990444579</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10</v>
       </c>
@@ -1784,7 +1798,7 @@
         <v>246500.25093327404</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>11</v>
       </c>
@@ -1816,39 +1830,47 @@
         <v>246143.4226553294</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="11">
         <v>12</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="12">
         <f t="shared" si="3"/>
         <v>260834.42907740417</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="12">
         <f t="shared" si="1"/>
         <v>4208.9566831089978</v>
       </c>
-      <c r="D21" s="9">
-        <v>1229.8499999999999</v>
-      </c>
-      <c r="E21" s="9">
+      <c r="D21" s="12">
+        <v>1229.8499999999999</v>
+      </c>
+      <c r="E21" s="12">
         <f t="shared" si="2"/>
         <v>1178.7650161350386</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="12">
         <f t="shared" si="4"/>
         <v>871.75795523762497</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="12">
         <f t="shared" si="0"/>
         <v>358.09204476237494</v>
       </c>
-      <c r="H21" s="9">
-        <f t="shared" si="5"/>
+      <c r="H21" s="12">
+        <f>H20-G21</f>
         <v>245785.33061056703</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J21" s="9">
+        <f>SUM(F10:F21)</f>
+        <v>10543.530610566999</v>
+      </c>
+      <c r="K21" s="9">
+        <f>SUM(G10:G21)</f>
+        <v>4214.669389433001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>13</v>
       </c>
@@ -1880,7 +1902,7 @@
         <v>245425.97032314612</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>14</v>
       </c>
@@ -1911,8 +1933,12 @@
         <f t="shared" si="5"/>
         <v>245065.33730137392</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J23" s="9">
+        <f>SUM(D10:D21)</f>
+        <v>14758.200000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>15</v>
       </c>
@@ -1944,7 +1970,7 @@
         <v>244703.42703764961</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>16</v>
       </c>
@@ -1976,7 +2002,7 @@
         <v>244340.23500840797</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>17</v>
       </c>
@@ -2008,7 +2034,7 @@
         <v>243975.75667406275</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>18</v>
       </c>
@@ -2040,7 +2066,7 @@
         <v>243609.98747895006</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>19</v>
       </c>
@@ -2072,7 +2098,7 @@
         <v>243242.92285127135</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>20</v>
       </c>
@@ -2104,7 +2130,7 @@
         <v>242874.55820303626</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>21</v>
       </c>
@@ -2136,7 +2162,7 @@
         <v>242504.88893000534</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>22</v>
       </c>
@@ -2168,7 +2194,7 @@
         <v>242133.91041163245</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>23</v>
       </c>
@@ -2200,39 +2226,39 @@
         <v>241761.61801100697</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="11">
         <v>24</v>
       </c>
-      <c r="B33" s="9">
+      <c r="B33" s="12">
         <f t="shared" si="3"/>
         <v>272138.39756854146</v>
       </c>
-      <c r="C33" s="9">
+      <c r="C33" s="12">
         <f t="shared" si="1"/>
         <v>4034.1268386198781</v>
       </c>
-      <c r="D33" s="9">
-        <v>1229.8499999999999</v>
-      </c>
-      <c r="E33" s="9">
+      <c r="D33" s="12">
+        <v>1229.8499999999999</v>
+      </c>
+      <c r="E33" s="12">
         <f t="shared" si="2"/>
         <v>1129.8019785045637</v>
       </c>
-      <c r="F33" s="9">
+      <c r="F33" s="12">
         <f t="shared" si="4"/>
         <v>856.23906378898312</v>
       </c>
-      <c r="G33" s="9">
+      <c r="G33" s="12">
         <f t="shared" si="0"/>
         <v>373.61093621101679</v>
       </c>
-      <c r="H33" s="9">
+      <c r="H33" s="12">
         <f t="shared" si="5"/>
         <v>241388.00707479595</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>25</v>
       </c>
@@ -2264,7 +2290,7 @@
         <v>241013.07293318585</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>26</v>
       </c>
@@ -2296,7 +2322,7 @@
         <v>240636.81089982422</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>27</v>
       </c>
@@ -2328,7 +2354,7 @@
         <v>240259.21627176111</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>28</v>
       </c>
@@ -2360,7 +2386,7 @@
         <v>239880.28432939027</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>29</v>
       </c>
@@ -2392,7 +2418,7 @@
         <v>239500.0103363902</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>30</v>
       </c>
@@ -2424,7 +2450,7 @@
         <v>239118.38953966493</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>31</v>
       </c>
@@ -2456,7 +2482,7 @@
         <v>238735.41716928457</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>32</v>
       </c>
@@ -2488,7 +2514,7 @@
         <v>238351.0884384258</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>33</v>
       </c>
@@ -2520,7 +2546,7 @@
         <v>237965.39854331189</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>34</v>
       </c>
@@ -2552,7 +2578,7 @@
         <v>237578.34266315278</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>35</v>
       </c>
@@ -2584,7 +2610,7 @@
         <v>237189.91596008479</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>36</v>
       </c>
@@ -2616,7 +2642,7 @@
         <v>236800.1135791101</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>37</v>
       </c>
@@ -2648,7 +2674,7 @@
         <v>236408.93064803613</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>38</v>
       </c>
@@ -2680,7 +2706,7 @@
         <v>236016.36227741459</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>39</v>
       </c>
@@ -2712,7 +2738,7 @@
         <v>235622.40356048042</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>40</v>
       </c>
@@ -2744,7 +2770,7 @@
         <v>235227.04957309045</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>41</v>
       </c>
@@ -2776,7 +2802,7 @@
         <v>234830.29537366182</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>42</v>
       </c>
@@ -2808,7 +2834,7 @@
         <v>234432.13600311021</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>43</v>
       </c>
@@ -2840,7 +2866,7 @@
         <v>234032.56648478788</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>44</v>
       </c>
@@ -2872,7 +2898,7 @@
         <v>233631.5818244215</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>45</v>
       </c>
@@ -2904,7 +2930,7 @@
         <v>233229.17701004967</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>46</v>
       </c>
@@ -2936,7 +2962,7 @@
         <v>232825.34701196026</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>47</v>
       </c>
@@ -2968,7 +2994,7 @@
         <v>232420.08678262762</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>48</v>
       </c>
@@ -3000,7 +3026,7 @@
         <v>232013.39125664943</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>49</v>
       </c>
@@ -3032,7 +3058,7 @@
         <v>231605.25535068338</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>50</v>
       </c>
@@ -3064,7 +3090,7 @@
         <v>231195.67396338371</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>51</v>
       </c>
@@ -3096,7 +3122,7 @@
         <v>230784.64197533738</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>52</v>
       </c>
@@ -3128,7 +3154,7 @@
         <v>230372.15424900004</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>53</v>
       </c>
@@ -3160,7 +3186,7 @@
         <v>229958.20562863193</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>54</v>
       </c>
@@ -3192,7 +3218,7 @@
         <v>229542.79094023333</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>55</v>
       </c>
@@ -3224,7 +3250,7 @@
         <v>229125.90499148</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>56</v>
       </c>
@@ -3256,7 +3282,7 @@
         <v>228707.54257165815</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>57</v>
       </c>
@@ -3288,7 +3314,7 @@
         <v>228287.69845159946</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>58</v>
       </c>
@@ -3320,7 +3346,7 @@
         <v>227866.36738361555</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>59</v>
       </c>
@@ -3352,7 +3378,7 @@
         <v>227443.54410143252</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>60</v>
       </c>
@@ -3384,7 +3410,7 @@
         <v>227019.22332012508</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>61</v>
       </c>
@@ -3416,7 +3442,7 @@
         <v>226593.39973605052</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>62</v>
       </c>
@@ -3448,7 +3474,7 @@
         <v>226166.06802678236</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>63</v>
       </c>
@@ -3480,7 +3506,7 @@
         <v>225737.22285104389</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>64</v>
       </c>
@@ -3512,7 +3538,7 @@
         <v>225306.85884864134</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>65</v>
       </c>
@@ -3536,7 +3562,7 @@
         <v>797.96179175560474</v>
       </c>
       <c r="G74" s="9">
-        <f t="shared" ref="G74:G105" si="7">D74-F74</f>
+        <f t="shared" ref="G74:G75" si="7">D74-F74</f>
         <v>431.88820824439517</v>
       </c>
       <c r="H74" s="9">
@@ -3544,7 +3570,7 @@
         <v>224874.97064039693</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>66</v>
       </c>
@@ -3576,7 +3602,7 @@
         <v>224441.55282808168</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>67</v>
       </c>
@@ -3608,7 +3634,7 @@
         <v>224006.59999434781</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>68</v>
       </c>
@@ -3640,7 +3666,7 @@
         <v>223570.10670266111</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>69</v>
       </c>
@@ -3672,7 +3698,7 @@
         <v>223132.06749723305</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>70</v>
       </c>
@@ -3704,7 +3730,7 @@
         <v>222692.47690295242</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>71</v>
       </c>
@@ -3736,7 +3762,7 @@
         <v>222251.32942531703</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>72</v>
       </c>
@@ -3768,7 +3794,7 @@
         <v>221808.61955036502</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>73</v>
       </c>
@@ -3800,7 +3826,7 @@
         <v>221364.34174460589</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>74</v>
       </c>
@@ -3832,7 +3858,7 @@
         <v>220918.49045495136</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>75</v>
       </c>
@@ -3864,7 +3890,7 @@
         <v>220471.06010864596</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>76</v>
       </c>
@@ -3896,7 +3922,7 @@
         <v>220022.04511319741</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>77</v>
       </c>
@@ -3928,7 +3954,7 @@
         <v>219571.43985630665</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>78</v>
       </c>
@@ -3960,7 +3986,7 @@
         <v>219119.23870579773</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>79</v>
       </c>
@@ -3992,7 +4018,7 @@
         <v>218665.43600954744</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>80</v>
       </c>
@@ -4024,7 +4050,7 @@
         <v>218210.02609541459</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>81</v>
       </c>
@@ -4056,7 +4082,7 @@
         <v>217753.00327116917</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>82</v>
       </c>
@@ -4088,7 +4114,7 @@
         <v>217294.36182442124</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>83</v>
       </c>
@@ -4120,7 +4146,7 @@
         <v>216834.09602254941</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>84</v>
       </c>
@@ -4152,7 +4178,7 @@
         <v>216372.20011262927</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>85</v>
       </c>
@@ -4184,7 +4210,7 @@
         <v>215908.6683213615</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>86</v>
       </c>
@@ -4216,7 +4242,7 @@
         <v>215443.49485499965</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>87</v>
       </c>
@@ -4248,7 +4274,7 @@
         <v>214976.67389927778</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>88</v>
       </c>
@@ -4280,7 +4306,7 @@
         <v>214508.19961933771</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>89</v>
       </c>
@@ -4312,7 +4338,7 @@
         <v>214038.06615965621</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>90</v>
       </c>
@@ -4344,7 +4370,7 @@
         <v>213566.26764397166</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>91</v>
       </c>
@@ -4376,7 +4402,7 @@
         <v>213092.79817521072</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>92</v>
       </c>
@@ -4408,7 +4434,7 @@
         <v>212617.65183541458</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>93</v>
       </c>
@@ -4440,7 +4466,7 @@
         <v>212140.82268566501</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>94</v>
       </c>
@@ -4472,7 +4498,7 @@
         <v>211662.30476601009</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>95</v>
       </c>
@@ -4504,7 +4530,7 @@
         <v>211182.0920953897</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>96</v>
       </c>
@@ -4536,7 +4562,7 @@
         <v>210700.17867156086</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>97</v>
       </c>
@@ -4568,7 +4594,7 @@
         <v>210216.55847102264</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>98</v>
       </c>
@@ -4600,7 +4626,7 @@
         <v>209731.22544894085</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>99</v>
       </c>
@@ -4632,7 +4658,7 @@
         <v>209244.17353907251</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>100</v>
       </c>
@@ -4664,7 +4690,7 @@
         <v>208755.39665369006</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>101</v>
       </c>
@@ -4696,7 +4722,7 @@
         <v>208264.88868350521</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>102</v>
       </c>
@@ -4728,7 +4754,7 @@
         <v>207772.64349759262</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>103</v>
       </c>
@@ -4760,7 +4786,7 @@
         <v>207278.65494331327</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>104</v>
       </c>
@@ -4792,7 +4818,7 @@
         <v>206782.91684623752</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>105</v>
       </c>
@@ -4824,7 +4850,7 @@
         <v>206285.42301006796</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>106</v>
       </c>
@@ -4856,7 +4882,7 @@
         <v>205786.16721656194</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>107</v>
       </c>
@@ -4888,7 +4914,7 @@
         <v>205285.14322545394</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>108</v>
       </c>
@@ -4920,7 +4946,7 @@
         <v>204782.34477437742</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>109</v>
       </c>
@@ -4952,7 +4978,7 @@
         <v>204277.76557878667</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>110</v>
       </c>
@@ -4984,7 +5010,7 @@
         <v>203771.3993318782</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>111</v>
       </c>
@@ -5016,7 +5042,7 @@
         <v>203263.23970451194</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>112</v>
       </c>
@@ -5048,7 +5074,7 @@
         <v>202753.28034513208</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>113</v>
       </c>
@@ -5080,7 +5106,7 @@
         <v>202241.51487968775</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>114</v>
       </c>
@@ -5112,7 +5138,7 @@
         <v>201727.93691155332</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>115</v>
       </c>
@@ -5144,7 +5170,7 @@
         <v>201212.5400214484</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>116</v>
       </c>
@@ -5176,7 +5202,7 @@
         <v>200695.31776735769</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>117</v>
       </c>
@@ -5208,7 +5234,7 @@
         <v>200176.26368445042</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>118</v>
       </c>
@@ -5240,7 +5266,7 @@
         <v>199655.37128499951</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>119</v>
       </c>
@@ -5272,7 +5298,7 @@
         <v>199132.63405830055</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>120</v>
       </c>
@@ -5304,7 +5330,7 @@
         <v>198608.04547059035</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>121</v>
       </c>
@@ -5336,7 +5362,7 @@
         <v>198081.59896496535</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>122</v>
       </c>
@@ -5368,7 +5394,7 @@
         <v>197553.28796129959</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>123</v>
       </c>
@@ -5400,7 +5426,7 @@
         <v>197023.10585616253</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>124</v>
       </c>
@@ -5432,7 +5458,7 @@
         <v>196491.04602273644</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>125</v>
       </c>
@@ -5464,7 +5490,7 @@
         <v>195957.10181073364</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>126</v>
       </c>
@@ -5496,7 +5522,7 @@
         <v>195421.26654631333</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>127</v>
       </c>
@@ -5528,7 +5554,7 @@
         <v>194883.5335319982</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>128</v>
       </c>
@@ -5560,7 +5586,7 @@
         <v>194343.8960465907</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>129</v>
       </c>
@@ -5592,7 +5618,7 @@
         <v>193802.34734508905</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>130</v>
       </c>
@@ -5624,7 +5650,7 @@
         <v>193258.88065860289</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>131</v>
       </c>
@@ -5656,7 +5682,7 @@
         <v>192713.48919426877</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>132</v>
       </c>
@@ -5688,7 +5714,7 @@
         <v>192166.16613516514</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>133</v>
       </c>
@@ -5720,7 +5746,7 @@
         <v>191616.90464022718</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>134</v>
       </c>
@@ -5752,7 +5778,7 @@
         <v>191065.6978441613</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>135</v>
       </c>
@@ -5784,7 +5810,7 @@
         <v>190512.53885735938</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>136</v>
       </c>
@@ -5816,7 +5842,7 @@
         <v>189957.42076581254</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>137</v>
       </c>
@@ -5848,7 +5874,7 @@
         <v>189400.33663102478</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>138</v>
       </c>
@@ -5880,7 +5906,7 @@
         <v>188841.27948992632</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>139</v>
       </c>
@@ -5912,7 +5938,7 @@
         <v>188280.24235478649</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>140</v>
       </c>
@@ -5944,7 +5970,7 @@
         <v>187717.21821312635</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>141</v>
       </c>
@@ -5976,7 +6002,7 @@
         <v>187152.20002763119</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>142</v>
       </c>
@@ -6008,7 +6034,7 @@
         <v>186585.18073606238</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>143</v>
       </c>
@@ -6040,7 +6066,7 @@
         <v>186016.15325116928</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>144</v>
       </c>
@@ -6072,7 +6098,7 @@
         <v>185445.1104606005</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>145</v>
       </c>
@@ -6104,7 +6130,7 @@
         <v>184872.04522681513</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>146</v>
       </c>
@@ -6136,7 +6162,7 @@
         <v>184296.95038699344</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>147</v>
       </c>
@@ -6168,7 +6194,7 @@
         <v>183719.81875294738</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>148</v>
       </c>
@@ -6200,7 +6226,7 @@
         <v>183140.64311103075</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>149</v>
       </c>
@@ -6232,7 +6258,7 @@
         <v>182559.41622204898</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>150</v>
       </c>
@@ -6264,7 +6290,7 @@
         <v>181976.13082116874</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>151</v>
       </c>
@@ -6296,7 +6322,7 @@
         <v>181390.77961782704</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>152</v>
       </c>
@@ -6328,7 +6354,7 @@
         <v>180803.35529564018</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>153</v>
       </c>
@@ -6360,7 +6386,7 @@
         <v>180213.85051231223</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>154</v>
       </c>
@@ -6392,7 +6418,7 @@
         <v>179622.25789954333</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>155</v>
       </c>
@@ -6424,7 +6450,7 @@
         <v>179028.57006293754</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>156</v>
       </c>
@@ -6456,7 +6482,7 @@
         <v>178432.77958191044</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>157</v>
       </c>
@@ -6488,7 +6514,7 @@
         <v>177834.87900959636</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>158</v>
       </c>
@@ -6520,7 +6546,7 @@
         <v>177234.86087275535</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>159</v>
       </c>
@@ -6552,7 +6578,7 @@
         <v>176632.71767167968</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>160</v>
       </c>
@@ -6584,7 +6610,7 @@
         <v>176028.4418801002</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>161</v>
       </c>
@@ -6616,7 +6642,7 @@
         <v>175422.02594509223</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>162</v>
       </c>
@@ -6648,7 +6674,7 @@
         <v>174813.46228698111</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>163</v>
       </c>
@@ -6680,7 +6706,7 @@
         <v>174202.74329924749</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>164</v>
       </c>
@@ -6712,7 +6738,7 @@
         <v>173589.86134843231</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>165</v>
       </c>
@@ -6744,7 +6770,7 @@
         <v>172974.80877404133</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>166</v>
       </c>
@@ -6776,7 +6802,7 @@
         <v>172357.57788844939</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>167</v>
       </c>
@@ -6808,7 +6834,7 @@
         <v>171738.16097680433</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>168</v>
       </c>
@@ -6840,7 +6866,7 @@
         <v>171116.55029693051</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>169</v>
       </c>
@@ -6872,7 +6898,7 @@
         <v>170492.73807923213</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>170</v>
       </c>
@@ -6904,7 +6930,7 @@
         <v>169866.71652659608</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>171</v>
       </c>
@@ -6936,7 +6962,7 @@
         <v>169238.47781429443</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>172</v>
       </c>
@@ -6968,7 +6994,7 @@
         <v>168608.01408988671</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>173</v>
       </c>
@@ -7000,7 +7026,7 @@
         <v>167975.31747312172</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>174</v>
       </c>
@@ -7032,7 +7058,7 @@
         <v>167340.38005583902</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>175</v>
       </c>
@@ -7064,7 +7090,7 @@
         <v>166703.19390187011</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>176</v>
       </c>
@@ -7096,7 +7122,7 @@
         <v>166063.75104693923</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>177</v>
       </c>
@@ -7128,7 +7154,7 @@
         <v>165422.04349856381</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>178</v>
       </c>
@@ -7160,7 +7186,7 @@
         <v>164778.06323595456</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>179</v>
       </c>
@@ -7192,7 +7218,7 @@
         <v>164131.80220991521</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>180</v>
       </c>
@@ -7224,7 +7250,7 @@
         <v>163483.25234274199</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>181</v>
       </c>
@@ -7256,7 +7282,7 @@
         <v>162832.40552812253</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>182</v>
       </c>
@@ -7288,7 +7314,7 @@
         <v>162179.25363103463</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>183</v>
       </c>
@@ -7320,7 +7346,7 @@
         <v>161523.78848764455</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>184</v>
       </c>
@@ -7352,7 +7378,7 @@
         <v>160866.00190520496</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>185</v>
       </c>
@@ -7384,7 +7410,7 @@
         <v>160205.88566195258</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>186</v>
       </c>
@@ -7416,7 +7442,7 @@
         <v>159543.43150700533</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>187</v>
       </c>
@@ -7448,7 +7474,7 @@
         <v>158878.63116025931</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>188</v>
       </c>
@@ -7480,7 +7506,7 @@
         <v>158211.47631228523</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>189</v>
       </c>
@@ -7512,7 +7538,7 @@
         <v>157541.95862422459</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>190</v>
       </c>
@@ -7544,7 +7570,7 @@
         <v>156870.06972768539</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>191</v>
       </c>
@@ -7576,7 +7602,7 @@
         <v>156195.8012246376</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>192</v>
       </c>
@@ -7608,7 +7634,7 @@
         <v>155519.1446873082</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>193</v>
       </c>
@@ -7640,7 +7666,7 @@
         <v>154840.09165807575</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>194</v>
       </c>
@@ -7672,7 +7698,7 @@
         <v>154158.63364936475</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>195</v>
       </c>
@@ -7704,7 +7730,7 @@
         <v>153474.76214353958</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>196</v>
       </c>
@@ -7736,7 +7762,7 @@
         <v>152788.46859279796</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>197</v>
       </c>
@@ -7768,7 +7794,7 @@
         <v>152099.74441906411</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>198</v>
       </c>
@@ -7800,7 +7826,7 @@
         <v>151408.58101388163</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>199</v>
       </c>
@@ -7832,7 +7858,7 @@
         <v>150714.96973830581</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>200</v>
       </c>
@@ -7864,7 +7890,7 @@
         <v>150018.90192279563</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>201</v>
       </c>
@@ -7896,7 +7922,7 @@
         <v>149320.36886710554</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>202</v>
       </c>
@@ -7928,7 +7954,7 @@
         <v>148619.36184017654</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>203</v>
       </c>
@@ -7960,7 +7986,7 @@
         <v>147915.87208002715</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>204</v>
       </c>
@@ -7992,7 +8018,7 @@
         <v>147209.89079364392</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>205</v>
       </c>
@@ -8024,7 +8050,7 @@
         <v>146501.40915687141</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>206</v>
       </c>
@@ -8056,7 +8082,7 @@
         <v>145790.41831430199</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>207</v>
       </c>
@@ -8088,7 +8114,7 @@
         <v>145076.90937916515</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>208</v>
       </c>
@@ -8120,7 +8146,7 @@
         <v>144360.87343321636</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>209</v>
       </c>
@@ -8152,7 +8178,7 @@
         <v>143642.30152662567</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>210</v>
       </c>
@@ -8184,7 +8210,7 @@
         <v>142921.18467786579</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>211</v>
       </c>
@@ -8216,7 +8242,7 @@
         <v>142197.51387359991</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>212</v>
       </c>
@@ -8248,7 +8274,7 @@
         <v>141471.28006856891</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>213</v>
       </c>
@@ -8280,7 +8306,7 @@
         <v>140742.47418547844</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>214</v>
       </c>
@@ -8312,7 +8338,7 @@
         <v>140011.08711488533</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>215</v>
       </c>
@@ -8344,7 +8370,7 @@
         <v>139277.10971508388</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>216</v>
       </c>
@@ -8376,7 +8402,7 @@
         <v>138540.53281199146</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>217</v>
       </c>
@@ -8408,7 +8434,7 @@
         <v>137801.34719903395</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>218</v>
       </c>
@@ -8440,7 +8466,7 @@
         <v>137059.54363703053</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>219</v>
       </c>
@@ -8472,7 +8498,7 @@
         <v>136315.11285407835</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>220</v>
       </c>
@@ -8504,7 +8530,7 @@
         <v>135568.04554543656</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>221</v>
       </c>
@@ -8536,7 +8562,7 @@
         <v>134818.33237340997</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>222</v>
       </c>
@@ -8568,7 +8594,7 @@
         <v>134065.96396723247</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>223</v>
       </c>
@@ -8600,7 +8626,7 @@
         <v>133310.93092294974</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>224</v>
       </c>
@@ -8632,7 +8658,7 @@
         <v>132553.22380330187</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>225</v>
       </c>
@@ -8664,7 +8690,7 @@
         <v>131792.83313760522</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>226</v>
       </c>
@@ -8696,7 +8722,7 @@
         <v>131029.74942163425</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>227</v>
       </c>
@@ -8728,7 +8754,7 @@
         <v>130263.96311750253</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>228</v>
       </c>
@@ -8760,7 +8786,7 @@
         <v>129495.46465354368</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>229</v>
       </c>
@@ -8792,7 +8818,7 @@
         <v>128724.24442419164</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>230</v>
       </c>
@@ -8824,7 +8850,7 @@
         <v>127950.29278986066</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>231</v>
       </c>
@@ -8856,7 +8882,7 @@
         <v>127173.60007682475</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>232</v>
       </c>
@@ -8888,7 +8914,7 @@
         <v>126394.15657709683</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>233</v>
       </c>
@@ -8920,7 +8946,7 @@
         <v>125611.95254830738</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>234</v>
       </c>
@@ -8952,7 +8978,7 @@
         <v>124826.97821358264</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>235</v>
       </c>
@@ -8984,7 +9010,7 @@
         <v>124039.22376142241</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>236</v>
       </c>
@@ -9016,7 +9042,7 @@
         <v>123248.67934557745</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>237</v>
       </c>
@@ -9048,7 +9074,7 @@
         <v>122455.33508492637</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>238</v>
       </c>
@@ -9080,7 +9106,7 @@
         <v>121659.18106335215</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>239</v>
       </c>
@@ -9112,7 +9138,7 @@
         <v>120860.20732961819</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>240</v>
       </c>
@@ -9144,7 +9170,7 @@
         <v>120058.40389724392</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>241</v>
       </c>
@@ -9176,7 +9202,7 @@
         <v>119253.76074437999</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>242</v>
       </c>
@@ -9208,7 +9234,7 @@
         <v>118446.26781368301</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>243</v>
       </c>
@@ -9240,7 +9266,7 @@
         <v>117635.9150121898</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>244</v>
       </c>
@@ -9272,7 +9298,7 @@
         <v>116822.6922111913</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>245</v>
       </c>
@@ -9304,7 +9330,7 @@
         <v>116006.58924610594</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>246</v>
       </c>
@@ -9336,7 +9362,7 @@
         <v>115187.59591635257</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>247</v>
       </c>
@@ -9368,7 +9394,7 @@
         <v>114365.70198522299</v>
       </c>
     </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>248</v>
       </c>
@@ -9400,7 +9426,7 @@
         <v>113540.89717975399</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>249</v>
       </c>
@@ -9432,7 +9458,7 @@
         <v>112713.17119059895</v>
       </c>
     </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>250</v>
       </c>
@@ -9464,7 +9490,7 @@
         <v>111882.51367189898</v>
       </c>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>251</v>
       </c>
@@ -9496,7 +9522,7 @@
         <v>111048.91424115363</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>252</v>
       </c>
@@ -9528,7 +9554,7 @@
         <v>110212.36247909105</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>253</v>
       </c>
@@ -9560,7 +9586,7 @@
         <v>109372.84792953783</v>
       </c>
     </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>254</v>
       </c>
@@ -9592,7 +9618,7 @@
         <v>108530.36009928829</v>
       </c>
     </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>255</v>
       </c>
@@ -9624,7 +9650,7 @@
         <v>107684.88845797327</v>
       </c>
     </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>256</v>
       </c>
@@ -9656,7 +9682,7 @@
         <v>106836.42243792859</v>
       </c>
     </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>257</v>
       </c>
@@ -9688,7 +9714,7 @@
         <v>105984.95143406292</v>
       </c>
     </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>258</v>
       </c>
@@ -9720,7 +9746,7 @@
         <v>105130.46480372523</v>
       </c>
     </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>259</v>
       </c>
@@ -9752,7 +9778,7 @@
         <v>104272.95186657176</v>
       </c>
     </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>260</v>
       </c>
@@ -9784,7 +9810,7 @@
         <v>103412.40190443254</v>
       </c>
     </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>261</v>
       </c>
@@ -9816,7 +9842,7 @@
         <v>102548.80416117741</v>
       </c>
     </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>262</v>
       </c>
@@ -9848,7 +9874,7 @@
         <v>101682.14784258157</v>
       </c>
     </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>263</v>
       </c>
@@ -9880,7 +9906,7 @@
         <v>100812.42211619072</v>
       </c>
     </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>264</v>
       </c>
@@ -9912,7 +9938,7 @@
         <v>99939.616111185562</v>
       </c>
     </row>
-    <row r="274" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>265</v>
       </c>
@@ -9944,7 +9970,7 @@
         <v>99063.718918246013</v>
       </c>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>266</v>
       </c>
@@ -9976,7 +10002,7 @@
         <v>98184.719589414803</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>267</v>
       </c>
@@ -10008,7 +10034,7 @@
         <v>97302.607137960644</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>268</v>
       </c>
@@ -10040,7 +10066,7 @@
         <v>96417.370538240924</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>269</v>
       </c>
@@ -10072,7 +10098,7 @@
         <v>95528.998725563855</v>
       </c>
     </row>
-    <row r="279" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>270</v>
       </c>
@@ -10104,7 +10130,7 @@
         <v>94637.480596050227</v>
       </c>
     </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>271</v>
       </c>
@@ -10136,7 +10162,7 @@
         <v>93742.805006494571</v>
       </c>
     </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>272</v>
       </c>
@@ -10168,7 +10194,7 @@
         <v>92844.96077422591</v>
       </c>
     </row>
-    <row r="282" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>273</v>
       </c>
@@ -10200,7 +10226,7 @@
         <v>91943.936676967962</v>
       </c>
     </row>
-    <row r="283" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>274</v>
       </c>
@@ -10232,7 +10258,7 @@
         <v>91039.721452698897</v>
       </c>
     </row>
-    <row r="284" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>275</v>
       </c>
@@ -10264,7 +10290,7 @@
         <v>90132.303799510541</v>
       </c>
     </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>276</v>
       </c>
@@ -10296,7 +10322,7 @@
         <v>89221.67237546714</v>
       </c>
     </row>
-    <row r="286" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>277</v>
       </c>
@@ -10328,7 +10354,7 @@
         <v>88307.815798463591</v>
       </c>
     </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>278</v>
       </c>
@@ -10360,7 +10386,7 @@
         <v>87390.722646083144</v>
       </c>
     </row>
-    <row r="288" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>279</v>
       </c>
@@ -10392,7 +10418,7 @@
         <v>86470.381455454684</v>
       </c>
     </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>280</v>
       </c>
@@ -10424,7 +10450,7 @@
         <v>85546.780723109419</v>
       </c>
     </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>281</v>
       </c>
@@ -10456,7 +10482,7 @@
         <v>84619.908904837095</v>
       </c>
     </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>282</v>
       </c>
@@ -10488,7 +10514,7 @@
         <v>83689.754415541727</v>
       </c>
     </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>283</v>
       </c>
@@ -10520,7 +10546,7 @@
         <v>82756.305629096765</v>
       </c>
     </row>
-    <row r="293" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>284</v>
       </c>
@@ -10552,7 +10578,7 @@
         <v>81819.550878199821</v>
       </c>
     </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>285</v>
       </c>
@@ -10584,7 +10610,7 @@
         <v>80879.478454226773</v>
       </c>
     </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>286</v>
       </c>
@@ -10616,7 +10642,7 @@
         <v>79936.076607085488</v>
       </c>
     </row>
-    <row r="296" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>287</v>
       </c>
@@ -10648,7 +10674,7 @@
         <v>78989.333545068919</v>
       </c>
     </row>
-    <row r="297" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>288</v>
       </c>
@@ -10680,7 +10706,7 @@
         <v>78039.237434707698</v>
       </c>
     </row>
-    <row r="298" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>289</v>
       </c>
@@ -10712,7 +10738,7 @@
         <v>77085.776400622286</v>
       </c>
     </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>290</v>
       </c>
@@ -10744,7 +10770,7 @@
         <v>76128.938525374484</v>
       </c>
     </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>291</v>
       </c>
@@ -10776,7 +10802,7 @@
         <v>75168.711849318512</v>
       </c>
     </row>
-    <row r="301" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>292</v>
       </c>
@@ -10808,7 +10834,7 @@
         <v>74205.084370451514</v>
       </c>
     </row>
-    <row r="302" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>293</v>
       </c>
@@ -10840,7 +10866,7 @@
         <v>73238.04404426353</v>
       </c>
     </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>294</v>
       </c>
@@ -10872,7 +10898,7 @@
         <v>72267.578783586971</v>
       </c>
     </row>
-    <row r="304" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>295</v>
       </c>
@@ -10904,7 +10930,7 @@
         <v>71293.676458445509</v>
       </c>
     </row>
-    <row r="305" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>296</v>
       </c>
@@ -10936,7 +10962,7 @@
         <v>70316.324895902508</v>
       </c>
     </row>
-    <row r="306" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>297</v>
       </c>
@@ -10968,7 +10994,7 @@
         <v>69335.511879908823</v>
       </c>
     </row>
-    <row r="307" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>298</v>
       </c>
@@ -11000,7 +11026,7 @@
         <v>68351.225151150167</v>
       </c>
     </row>
-    <row r="308" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>299</v>
       </c>
@@ -11032,7 +11058,7 @@
         <v>67363.452406893819</v>
       </c>
     </row>
-    <row r="309" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>300</v>
       </c>
@@ -11064,7 +11090,7 @@
         <v>66372.181300834898</v>
       </c>
     </row>
-    <row r="310" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>301</v>
       </c>
@@ -11096,7 +11122,7 @@
         <v>65377.39944294202</v>
       </c>
     </row>
-    <row r="311" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>302</v>
       </c>
@@ -11128,7 +11154,7 @@
         <v>64379.094399302441</v>
       </c>
     </row>
-    <row r="312" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>303</v>
       </c>
@@ -11160,7 +11186,7 @@
         <v>63377.253691966638</v>
       </c>
     </row>
-    <row r="313" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>304</v>
       </c>
@@ -11192,7 +11218,7 @@
         <v>62371.864798792354</v>
       </c>
     </row>
-    <row r="314" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>305</v>
       </c>
@@ -11224,7 +11250,7 @@
         <v>61362.915153288079</v>
       </c>
     </row>
-    <row r="315" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>306</v>
       </c>
@@ -11256,7 +11282,7 @@
         <v>60350.392144455975</v>
       </c>
     </row>
-    <row r="316" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>307</v>
       </c>
@@ -11288,7 +11314,7 @@
         <v>59334.283116634258</v>
       </c>
     </row>
-    <row r="317" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>308</v>
       </c>
@@ -11320,7 +11346,7 @@
         <v>58314.575369339007</v>
       </c>
     </row>
-    <row r="318" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>309</v>
       </c>
@@ -11352,7 +11378,7 @@
         <v>57291.256157105418</v>
       </c>
     </row>
-    <row r="319" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>310</v>
       </c>
@@ -11384,7 +11410,7 @@
         <v>56264.312689328501</v>
       </c>
     </row>
-    <row r="320" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>311</v>
       </c>
@@ -11416,7 +11442,7 @@
         <v>55233.732130103206</v>
       </c>
     </row>
-    <row r="321" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>312</v>
       </c>
@@ -11448,7 +11474,7 @@
         <v>54199.501598063987</v>
       </c>
     </row>
-    <row r="322" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>313</v>
       </c>
@@ -11480,7 +11506,7 @@
         <v>53161.608166223799</v>
       </c>
     </row>
-    <row r="323" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>314</v>
       </c>
@@ -11512,7 +11538,7 @@
         <v>52120.038861812507</v>
       </c>
     </row>
-    <row r="324" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>315</v>
       </c>
@@ -11544,7 +11570,7 @@
         <v>51074.780666114762</v>
       </c>
     </row>
-    <row r="325" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>316</v>
       </c>
@@ -11576,7 +11602,7 @@
         <v>50025.820514307256</v>
       </c>
     </row>
-    <row r="326" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>317</v>
       </c>
@@ -11608,7 +11634,7 @@
         <v>48973.145295295428</v>
       </c>
     </row>
-    <row r="327" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>318</v>
       </c>
@@ -11640,7 +11666,7 @@
         <v>47916.741851549596</v>
       </c>
     </row>
-    <row r="328" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>319</v>
       </c>
@@ -11672,7 +11698,7 @@
         <v>46856.596978940499</v>
       </c>
     </row>
-    <row r="329" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>320</v>
       </c>
@@ -11704,7 +11730,7 @@
         <v>45792.697426574246</v>
       </c>
     </row>
-    <row r="330" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>321</v>
       </c>
@@ -11736,7 +11762,7 @@
         <v>44725.0298966267</v>
       </c>
     </row>
-    <row r="331" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>322</v>
       </c>
@@ -11768,7 +11794,7 @@
         <v>43653.581044177256</v>
       </c>
     </row>
-    <row r="332" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>323</v>
       </c>
@@ -11800,7 +11826,7 @@
         <v>42578.337477042049</v>
       </c>
     </row>
-    <row r="333" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>324</v>
       </c>
@@ -11832,7 +11858,7 @@
         <v>41499.285755606572</v>
       </c>
     </row>
-    <row r="334" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>325</v>
       </c>
@@ -11864,7 +11890,7 @@
         <v>40416.412392657679</v>
       </c>
     </row>
-    <row r="335" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>326</v>
       </c>
@@ -11896,7 +11922,7 @@
         <v>39329.703853215011</v>
       </c>
     </row>
-    <row r="336" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>327</v>
       </c>
@@ -11928,7 +11954,7 @@
         <v>38239.146554361811</v>
       </c>
     </row>
-    <row r="337" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>328</v>
       </c>
@@ -11960,7 +11986,7 @@
         <v>37144.726865075172</v>
       </c>
     </row>
-    <row r="338" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>329</v>
       </c>
@@ -11992,7 +12018,7 @@
         <v>36046.43110605565</v>
       </c>
     </row>
-    <row r="339" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>330</v>
       </c>
@@ -12024,7 +12050,7 @@
         <v>34944.245549556261</v>
       </c>
     </row>
-    <row r="340" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>331</v>
       </c>
@@ -12056,7 +12082,7 @@
         <v>33838.156419210936</v>
       </c>
     </row>
-    <row r="341" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>332</v>
       </c>
@@ -12088,7 +12114,7 @@
         <v>32728.14988986231</v>
       </c>
     </row>
-    <row r="342" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>333</v>
       </c>
@@ -12120,7 +12146,7 @@
         <v>31614.212087388907</v>
       </c>
     </row>
-    <row r="343" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>334</v>
       </c>
@@ -12152,7 +12178,7 @@
         <v>30496.329088531744</v>
       </c>
     </row>
-    <row r="344" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>335</v>
       </c>
@@ -12184,7 +12210,7 @@
         <v>29374.486920720294</v>
       </c>
     </row>
-    <row r="345" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>336</v>
       </c>
@@ -12216,7 +12242,7 @@
         <v>28248.671561897845</v>
       </c>
     </row>
-    <row r="346" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>337</v>
       </c>
@@ -12248,7 +12274,7 @@
         <v>27118.868940346234</v>
       </c>
     </row>
-    <row r="347" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>338</v>
       </c>
@@ -12280,7 +12306,7 @@
         <v>25985.064934509959</v>
       </c>
     </row>
-    <row r="348" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>339</v>
       </c>
@@ -12312,7 +12338,7 @@
         <v>24847.245372819682</v>
       </c>
     </row>
-    <row r="349" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>340</v>
       </c>
@@ -12344,7 +12370,7 @@
         <v>23705.396033515084</v>
       </c>
     </row>
-    <row r="350" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>341</v>
       </c>
@@ -12376,7 +12402,7 @@
         <v>22559.502644467117</v>
       </c>
     </row>
-    <row r="351" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>342</v>
       </c>
@@ -12408,7 +12434,7 @@
         <v>21409.550882999603</v>
       </c>
     </row>
-    <row r="352" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A352">
         <v>343</v>
       </c>
@@ -12440,7 +12466,7 @@
         <v>20255.526375710226</v>
       </c>
     </row>
-    <row r="353" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A353">
         <v>344</v>
       </c>
@@ -12472,7 +12498,7 @@
         <v>19097.414698290868</v>
       </c>
     </row>
-    <row r="354" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>345</v>
       </c>
@@ -12504,7 +12530,7 @@
         <v>17935.201375347315</v>
       </c>
     </row>
-    <row r="355" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>346</v>
       </c>
@@ -12536,7 +12562,7 @@
         <v>16768.871880218336</v>
       </c>
     </row>
-    <row r="356" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>347</v>
       </c>
@@ -12568,7 +12594,7 @@
         <v>15598.411634794109</v>
       </c>
     </row>
-    <row r="357" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>348</v>
       </c>
@@ -12600,7 +12626,7 @@
         <v>14423.806009334005</v>
       </c>
     </row>
-    <row r="358" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>349</v>
       </c>
@@ -12632,7 +12658,7 @@
         <v>13245.040322283729</v>
       </c>
     </row>
-    <row r="359" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>350</v>
       </c>
@@ -12664,7 +12690,7 @@
         <v>12062.099840091816</v>
       </c>
     </row>
-    <row r="360" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A360">
         <v>351</v>
       </c>
@@ -12696,7 +12722,7 @@
         <v>10874.969777025475</v>
       </c>
     </row>
-    <row r="361" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A361">
         <v>352</v>
       </c>
@@ -12728,7 +12754,7 @@
         <v>9683.6352949857737</v>
       </c>
     </row>
-    <row r="362" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A362">
         <v>353</v>
       </c>
@@ -12760,7 +12786,7 @@
         <v>8488.0815033221825</v>
       </c>
     </row>
-    <row r="363" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A363">
         <v>354</v>
       </c>
@@ -12792,7 +12818,7 @@
         <v>7288.2934586464489</v>
       </c>
     </row>
-    <row r="364" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A364">
         <v>355</v>
       </c>
@@ -12824,7 +12850,7 @@
         <v>6084.2561646458216</v>
       </c>
     </row>
-    <row r="365" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A365">
         <v>356</v>
       </c>
@@ -12856,7 +12882,7 @@
         <v>4875.9545718956088</v>
       </c>
     </row>
-    <row r="366" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A366">
         <v>357</v>
       </c>
@@ -12888,7 +12914,7 @@
         <v>3663.3735776710728</v>
       </c>
     </row>
-    <row r="367" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A367">
         <v>358</v>
       </c>
@@ -12920,7 +12946,7 @@
         <v>2446.4980257586576</v>
       </c>
     </row>
-    <row r="368" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A368">
         <v>359</v>
       </c>
@@ -12952,7 +12978,7 @@
         <v>1225.3127062665531</v>
       </c>
     </row>
-    <row r="369" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A369">
         <v>360</v>
       </c>

</xml_diff>